<commit_message>
Updated Beaglebone pinout document
Updated Beaglebone pinout document.
</commit_message>
<xml_diff>
--- a/Supporting Documents/BeagleBone/Beaglebone connectors.xlsx
+++ b/Supporting Documents/BeagleBone/Beaglebone connectors.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="555">
   <si>
     <t>Beaglebone P8</t>
   </si>
@@ -1660,6 +1660,27 @@
   </si>
   <si>
     <t>gpio3_18</t>
+  </si>
+  <si>
+    <t>analog</t>
+  </si>
+  <si>
+    <t>GPMC</t>
+  </si>
+  <si>
+    <t>UART</t>
+  </si>
+  <si>
+    <t>I2C</t>
+  </si>
+  <si>
+    <t>SPI</t>
+  </si>
+  <si>
+    <t>eMMC</t>
+  </si>
+  <si>
+    <t>GPIO</t>
   </si>
 </sst>
 </file>
@@ -1675,7 +1696,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1685,12 +1706,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1724,6 +1739,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1737,11 +1764,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1767,7 +1791,16 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1778,9 +1811,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF3399"/>
       <color rgb="FF808000"/>
       <color rgb="FFFF6699"/>
-      <color rgb="FFFF3399"/>
       <color rgb="FFFFCCCC"/>
       <color rgb="FFFFFFCC"/>
     </mruColors>
@@ -2080,2841 +2113,2892 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N99"/>
+  <dimension ref="A1:N109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="28.77734375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="21.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="12.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="21.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="2"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>2</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>3</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>4</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="2">
         <v>5</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="2">
         <v>6</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
+    <row r="5" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="M5" s="5" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
+    <row r="6" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="M6" s="5" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
+    <row r="7" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="M7" s="5" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+    <row r="8" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="M8" s="5" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+    <row r="9" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="D9" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="M9" s="13" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+    <row r="10" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="D10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="M10" s="3" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+    <row r="11" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="D11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="M11" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+    <row r="12" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="4" t="s">
+      <c r="D12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+    <row r="13" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="4" t="s">
+      <c r="D13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L13" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="M13" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
+    <row r="14" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="4" t="s">
+      <c r="D14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
+    <row r="15" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
         <v>13</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="4" t="s">
+      <c r="D15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="M15" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+    <row r="16" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
         <v>14</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="4" t="s">
+      <c r="D16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="M16" s="3" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
+    <row r="17" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
         <v>15</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="4" t="s">
+      <c r="D17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="L17" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="M17" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
+    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
         <v>16</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="4" t="s">
+      <c r="D18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="L18" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="M18" s="4" t="s">
+      <c r="M18" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
+    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
         <v>17</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="4" t="s">
+      <c r="D19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="M19" s="3" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+    <row r="20" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13">
         <v>18</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="3" t="s">
+      <c r="D20" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="J20" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="K20" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="L20" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="M20" s="3" t="s">
+      <c r="M20" s="13" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
+    <row r="21" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
         <v>19</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="4" t="s">
+      <c r="D21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H21" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="I21" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="M21" s="4" t="s">
+      <c r="M21" s="3" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
+    <row r="22" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
         <v>20</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="5" t="s">
         <v>433</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="H22" s="5" t="s">
         <v>434</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="I22" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="J22" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="K22" s="7" t="s">
+      <c r="K22" s="5" t="s">
         <v>435</v>
       </c>
-      <c r="L22" s="7" t="s">
+      <c r="L22" s="5" t="s">
         <v>436</v>
       </c>
-      <c r="M22" s="7" t="s">
+      <c r="M22" s="5" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7">
+    <row r="23" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
         <v>21</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="H23" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="I23" s="7" t="s">
+      <c r="I23" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="J23" s="7" t="s">
+      <c r="J23" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="K23" s="7" t="s">
+      <c r="K23" s="5" t="s">
         <v>430</v>
       </c>
-      <c r="L23" s="7" t="s">
+      <c r="L23" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="M23" s="7" t="s">
+      <c r="M23" s="5" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6">
+    <row r="24" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
         <v>22</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>426</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="M24" s="6" t="s">
+      <c r="M24" s="5" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="6">
+    <row r="25" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
         <v>23</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>424</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="M25" s="6" t="s">
+      <c r="M25" s="5" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6">
+    <row r="26" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
         <v>24</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>422</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="G26" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="M26" s="6" t="s">
+      <c r="M26" s="5" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="6">
+    <row r="27" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
         <v>25</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="M27" s="6" t="s">
+      <c r="M27" s="5" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
+    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
         <v>26</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F28" s="4" t="s">
+      <c r="D28" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="M28" s="4" t="s">
+      <c r="M28" s="3" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4">
+    <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
         <v>27</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="4" t="s">
+      <c r="D29" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="I29" s="4" t="s">
+      <c r="I29" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="J29" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="K29" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="L29" s="4" t="s">
+      <c r="L29" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="M29" s="4" t="s">
+      <c r="M29" s="3" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4">
+    <row r="30" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
         <v>28</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F30" s="4" t="s">
+      <c r="D30" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="G30" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="H30" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="I30" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="J30" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="K30" s="4" t="s">
+      <c r="K30" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="L30" s="4" t="s">
+      <c r="L30" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="M30" s="4" t="s">
+      <c r="M30" s="3" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4">
+    <row r="31" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
         <v>29</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F31" s="4" t="s">
+      <c r="D31" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="G31" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="H31" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="I31" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="J31" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="K31" s="4" t="s">
+      <c r="K31" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="L31" s="4" t="s">
+      <c r="L31" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="M31" s="4" t="s">
+      <c r="M31" s="3" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4">
+    <row r="32" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
         <v>30</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F32" s="4" t="s">
+      <c r="D32" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G32" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="H32" s="4" t="s">
+      <c r="H32" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I32" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="J32" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="K32" s="4" t="s">
+      <c r="K32" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="L32" s="4" t="s">
+      <c r="L32" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="M32" s="4" t="s">
+      <c r="M32" s="3" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4">
+    <row r="33" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
         <v>31</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F33" s="4" t="s">
+      <c r="D33" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="G33" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="H33" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="I33" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="J33" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="K33" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="L33" s="4" t="s">
+      <c r="L33" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="M33" s="4" t="s">
+      <c r="M33" s="3" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="4">
+    <row r="34" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
         <v>32</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F34" s="4" t="s">
+      <c r="D34" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="G34" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="H34" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="I34" s="4" t="s">
+      <c r="I34" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="J34" s="4" t="s">
+      <c r="J34" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="K34" s="4" t="s">
+      <c r="K34" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="L34" s="4" t="s">
+      <c r="L34" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="M34" s="4" t="s">
+      <c r="M34" s="3" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4">
+    <row r="35" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
         <v>33</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F35" s="4" t="s">
+      <c r="D35" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="G35" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="H35" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="I35" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="J35" s="4" t="s">
+      <c r="J35" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="K35" s="4" t="s">
+      <c r="K35" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="L35" s="4" t="s">
+      <c r="L35" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="M35" s="4" t="s">
+      <c r="M35" s="3" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="4">
+    <row r="36" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
         <v>34</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F36" s="4" t="s">
+      <c r="D36" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G36" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="H36" s="4" t="s">
+      <c r="H36" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="I36" s="4" t="s">
+      <c r="I36" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="J36" s="4" t="s">
+      <c r="J36" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="K36" s="4" t="s">
+      <c r="K36" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="L36" s="4" t="s">
+      <c r="L36" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="M36" s="4" t="s">
+      <c r="M36" s="3" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="4">
+    <row r="37" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
         <v>35</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F37" s="4" t="s">
+      <c r="D37" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G37" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="H37" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="I37" s="4" t="s">
+      <c r="I37" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="J37" s="4" t="s">
+      <c r="J37" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="K37" s="4" t="s">
+      <c r="K37" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="L37" s="4" t="s">
+      <c r="L37" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="M37" s="4" t="s">
+      <c r="M37" s="3" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="4">
+    <row r="38" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
         <v>36</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F38" s="4" t="s">
+      <c r="D38" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G38" s="4" t="s">
+      <c r="G38" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="H38" s="4" t="s">
+      <c r="H38" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="I38" s="4" t="s">
+      <c r="I38" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="K38" s="4" t="s">
+      <c r="K38" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="L38" s="4" t="s">
+      <c r="L38" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="M38" s="4" t="s">
+      <c r="M38" s="3" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="4">
+    <row r="39" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
         <v>37</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F39" s="4" t="s">
+      <c r="D39" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="G39" s="4" t="s">
+      <c r="G39" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="H39" s="4" t="s">
+      <c r="H39" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="I39" s="4" t="s">
+      <c r="I39" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="J39" s="4" t="s">
+      <c r="J39" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="K39" s="4" t="s">
+      <c r="K39" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="L39" s="4" t="s">
+      <c r="L39" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="M39" s="4" t="s">
+      <c r="M39" s="3" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="4">
+    <row r="40" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
         <v>38</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F40" s="4" t="s">
+      <c r="D40" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="G40" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="H40" s="4" t="s">
+      <c r="H40" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="I40" s="4" t="s">
+      <c r="I40" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="J40" s="4" t="s">
+      <c r="J40" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="K40" s="4" t="s">
+      <c r="K40" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="L40" s="4" t="s">
+      <c r="L40" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="M40" s="4" t="s">
+      <c r="M40" s="3" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4">
+    <row r="41" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
         <v>39</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F41" s="4" t="s">
+      <c r="D41" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="G41" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="H41" s="4" t="s">
+      <c r="H41" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="I41" s="4" t="s">
+      <c r="I41" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="J41" s="4" t="s">
+      <c r="J41" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="K41" s="4" t="s">
+      <c r="K41" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="L41" s="4" t="s">
+      <c r="L41" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="M41" s="4" t="s">
+      <c r="M41" s="3" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="4">
+    <row r="42" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
         <v>40</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F42" s="4" t="s">
+      <c r="D42" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="G42" s="4" t="s">
+      <c r="G42" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="H42" s="4" t="s">
+      <c r="H42" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="I42" s="4" t="s">
+      <c r="I42" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="J42" s="4" t="s">
+      <c r="J42" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="K42" s="4" t="s">
+      <c r="K42" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="L42" s="4" t="s">
+      <c r="L42" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="M42" s="4" t="s">
+      <c r="M42" s="3" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="4">
+    <row r="43" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
         <v>41</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F43" s="4" t="s">
+      <c r="D43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="G43" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="H43" s="4" t="s">
+      <c r="H43" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="I43" s="4" t="s">
+      <c r="I43" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="K43" s="4" t="s">
+      <c r="K43" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="L43" s="4" t="s">
+      <c r="L43" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="M43" s="4" t="s">
+      <c r="M43" s="3" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="4">
+    <row r="44" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
         <v>42</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F44" s="4" t="s">
+      <c r="D44" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="G44" s="4" t="s">
+      <c r="G44" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="H44" s="4" t="s">
+      <c r="H44" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="I44" s="4" t="s">
+      <c r="I44" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="K44" s="4" t="s">
+      <c r="K44" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="L44" s="4" t="s">
+      <c r="L44" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="M44" s="4" t="s">
+      <c r="M44" s="3" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="4">
+    <row r="45" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
         <v>43</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F45" s="4" t="s">
+      <c r="D45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="G45" s="4" t="s">
+      <c r="G45" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="H45" s="4" t="s">
+      <c r="H45" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="I45" s="4" t="s">
+      <c r="I45" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="K45" s="4" t="s">
+      <c r="K45" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="L45" s="4" t="s">
+      <c r="L45" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="M45" s="4" t="s">
+      <c r="M45" s="3" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="4">
+    <row r="46" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
         <v>44</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F46" s="4" t="s">
+      <c r="D46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="G46" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="H46" s="4" t="s">
+      <c r="H46" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="I46" s="4" t="s">
+      <c r="I46" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="K46" s="4" t="s">
+      <c r="K46" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="L46" s="4" t="s">
+      <c r="L46" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="M46" s="4" t="s">
+      <c r="M46" s="3" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4">
+    <row r="47" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="3">
         <v>45</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D47" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F47" s="4" t="s">
+      <c r="D47" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="G47" s="4" t="s">
+      <c r="G47" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="H47" s="4" t="s">
+      <c r="H47" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="I47" s="4" t="s">
+      <c r="I47" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K47" s="4" t="s">
+      <c r="K47" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="L47" s="4" t="s">
+      <c r="L47" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="M47" s="4" t="s">
+      <c r="M47" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="48" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="4">
+    <row r="48" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="3">
         <v>46</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F48" s="4" t="s">
+      <c r="D48" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="G48" s="4" t="s">
+      <c r="G48" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="H48" s="4" t="s">
+      <c r="H48" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="I48" s="4" t="s">
+      <c r="I48" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="K48" s="4" t="s">
+      <c r="K48" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="L48" s="4" t="s">
+      <c r="L48" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="M48" s="4" t="s">
+      <c r="M48" s="3" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E51" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A52" s="3">
+      <c r="A52" s="2">
         <v>1</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A53" s="3">
+      <c r="A53" s="2">
         <v>2</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A54" s="3">
+      <c r="A54" s="2">
         <v>3</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A55" s="3">
+      <c r="A55" s="2">
         <v>4</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A56" s="3">
+      <c r="A56" s="2">
         <v>5</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A57" s="3">
+      <c r="A57" s="2">
         <v>6</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A58" s="3">
+      <c r="A58" s="2">
         <v>7</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A59" s="3">
+      <c r="A59" s="2">
         <v>8</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A60" s="3">
+      <c r="A60" s="2">
         <v>9</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E60" s="2" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A61" s="3">
+      <c r="A61" s="2">
         <v>10</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E61" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="F61" s="2" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="62" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="4">
+    <row r="62" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="3">
         <v>11</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D62" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F62" s="4" t="s">
+      <c r="D62" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F62" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="G62" s="4" t="s">
+      <c r="G62" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="H62" s="4" t="s">
+      <c r="H62" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="I62" s="4" t="s">
+      <c r="I62" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="J62" s="4" t="s">
+      <c r="J62" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="K62" s="4" t="s">
+      <c r="K62" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="L62" s="4" t="s">
+      <c r="L62" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="M62" s="4" t="s">
+      <c r="M62" s="3" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="63" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="4">
+    <row r="63" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="3">
         <v>12</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C63" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D63" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F63" s="4" t="s">
+      <c r="D63" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F63" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="G63" s="4" t="s">
+      <c r="G63" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="H63" s="4" t="s">
+      <c r="H63" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="I63" s="4" t="s">
+      <c r="I63" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="J63" s="4" t="s">
+      <c r="J63" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="K63" s="4" t="s">
+      <c r="K63" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="L63" s="4" t="s">
+      <c r="L63" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="M63" s="4" t="s">
+      <c r="M63" s="3" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A64" s="3">
+    <row r="64" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="13">
         <v>13</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F64" s="3" t="s">
+      <c r="D64" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F64" s="13" t="s">
         <v>408</v>
       </c>
-      <c r="G64" s="3" t="s">
+      <c r="G64" s="13" t="s">
         <v>409</v>
       </c>
-      <c r="H64" s="3" t="s">
+      <c r="H64" s="13" t="s">
         <v>410</v>
       </c>
-      <c r="I64" s="3" t="s">
+      <c r="I64" s="13" t="s">
         <v>411</v>
       </c>
-      <c r="J64" s="3" t="s">
+      <c r="J64" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="K64" s="3" t="s">
+      <c r="K64" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="L64" s="3" t="s">
+      <c r="L64" s="13" t="s">
         <v>414</v>
       </c>
-      <c r="M64" s="3" t="s">
+      <c r="M64" s="13" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A65" s="3">
+    <row r="65" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="13">
         <v>14</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F65" s="3" t="s">
+      <c r="D65" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F65" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="G65" s="3" t="s">
+      <c r="G65" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="H65" s="3" t="s">
+      <c r="H65" s="13" t="s">
         <v>417</v>
       </c>
-      <c r="I65" s="3" t="s">
+      <c r="I65" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="J65" s="3" t="s">
+      <c r="J65" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="K65" s="3" t="s">
+      <c r="K65" s="13" t="s">
         <v>418</v>
       </c>
-      <c r="L65" s="3" t="s">
+      <c r="L65" s="13" t="s">
         <v>332</v>
       </c>
-      <c r="M65" s="3" t="s">
+      <c r="M65" s="13" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="66" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="4">
+    <row r="66" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="3">
         <v>15</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D66" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F66" s="4" t="s">
+      <c r="D66" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F66" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="G66" s="4" t="s">
+      <c r="G66" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="H66" s="4" t="s">
+      <c r="H66" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="I66" s="4" t="s">
+      <c r="I66" s="3" t="s">
         <v>440</v>
       </c>
-      <c r="J66" s="4" t="s">
+      <c r="J66" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="K66" s="4" t="s">
+      <c r="K66" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="L66" s="4" t="s">
+      <c r="L66" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="M66" s="4" t="s">
+      <c r="M66" s="3" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="67" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C67" s="4" t="s">
+    <row r="67" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C67" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="F67" s="4" t="s">
+      <c r="F67" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="G67" s="4" t="s">
+      <c r="G67" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="H67" s="4" t="s">
+      <c r="H67" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="I67" s="4" t="s">
+      <c r="I67" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="J67" s="4" t="s">
+      <c r="J67" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="K67" s="4" t="s">
+      <c r="K67" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="L67" s="4" t="s">
+      <c r="L67" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="M67" s="4" t="s">
+      <c r="M67" s="3" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A68" s="3">
+    <row r="68" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="13">
         <v>16</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F68" s="3" t="s">
+      <c r="D68" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F68" s="13" t="s">
         <v>380</v>
       </c>
-      <c r="G68" s="3" t="s">
+      <c r="G68" s="13" t="s">
         <v>448</v>
       </c>
-      <c r="H68" s="3" t="s">
+      <c r="H68" s="13" t="s">
         <v>449</v>
       </c>
-      <c r="I68" s="3" t="s">
+      <c r="I68" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="J68" s="3" t="s">
+      <c r="J68" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="K68" s="3" t="s">
+      <c r="K68" s="13" t="s">
         <v>450</v>
       </c>
-      <c r="L68" s="3" t="s">
+      <c r="L68" s="13" t="s">
         <v>317</v>
       </c>
-      <c r="M68" s="3" t="s">
+      <c r="M68" s="13" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="69" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="9">
+    <row r="69" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="7">
         <v>17</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="B69" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C69" s="9" t="s">
+      <c r="C69" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="D69" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F69" s="9" t="s">
+      <c r="D69" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F69" s="7" t="s">
         <v>452</v>
       </c>
-      <c r="G69" s="9" t="s">
+      <c r="G69" s="7" t="s">
         <v>453</v>
       </c>
-      <c r="H69" s="9" t="s">
+      <c r="H69" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="I69" s="9" t="s">
+      <c r="I69" s="7" t="s">
         <v>454</v>
       </c>
-      <c r="J69" s="9" t="s">
+      <c r="J69" s="7" t="s">
         <v>455</v>
       </c>
-      <c r="K69" s="9" t="s">
+      <c r="K69" s="7" t="s">
         <v>456</v>
       </c>
-      <c r="L69" s="9" t="s">
+      <c r="L69" s="7" t="s">
         <v>457</v>
       </c>
-      <c r="M69" s="9" t="s">
+      <c r="M69" s="7" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="70" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="9">
+    <row r="70" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="7">
         <v>18</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="B70" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C70" s="9" t="s">
+      <c r="C70" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D70" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F70" s="9" t="s">
+      <c r="D70" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F70" s="7" t="s">
         <v>459</v>
       </c>
-      <c r="G70" s="9" t="s">
+      <c r="G70" s="7" t="s">
         <v>460</v>
       </c>
-      <c r="H70" s="9" t="s">
+      <c r="H70" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="I70" s="9" t="s">
+      <c r="I70" s="7" t="s">
         <v>461</v>
       </c>
-      <c r="J70" s="9" t="s">
+      <c r="J70" s="7" t="s">
         <v>462</v>
       </c>
-      <c r="K70" s="9" t="s">
+      <c r="K70" s="7" t="s">
         <v>463</v>
       </c>
-      <c r="L70" s="9" t="s">
+      <c r="L70" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="M70" s="9" t="s">
+      <c r="M70" s="7" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="71" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="10">
+    <row r="71" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="8">
         <v>19</v>
       </c>
-      <c r="B71" s="10" t="s">
+      <c r="B71" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C71" s="10" t="s">
+      <c r="C71" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D71" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F71" s="10" t="s">
+      <c r="D71" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F71" s="8" t="s">
         <v>466</v>
       </c>
-      <c r="G71" s="10" t="s">
+      <c r="G71" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="H71" s="10" t="s">
+      <c r="H71" s="8" t="s">
         <v>467</v>
       </c>
-      <c r="I71" s="10" t="s">
+      <c r="I71" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="J71" s="10" t="s">
+      <c r="J71" s="8" t="s">
         <v>468</v>
       </c>
-      <c r="K71" s="10" t="s">
+      <c r="K71" s="8" t="s">
         <v>469</v>
       </c>
-      <c r="L71" s="10" t="s">
+      <c r="L71" s="8" t="s">
         <v>470</v>
       </c>
-      <c r="M71" s="10" t="s">
+      <c r="M71" s="8" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="72" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="10">
+    <row r="72" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="8">
         <v>20</v>
       </c>
-      <c r="B72" s="10" t="s">
+      <c r="B72" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C72" s="10" t="s">
+      <c r="C72" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D72" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F72" s="10" t="s">
+      <c r="D72" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F72" s="8" t="s">
         <v>472</v>
       </c>
-      <c r="G72" s="10" t="s">
+      <c r="G72" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="H72" s="10" t="s">
+      <c r="H72" s="8" t="s">
         <v>473</v>
       </c>
-      <c r="I72" s="10" t="s">
+      <c r="I72" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="J72" s="10" t="s">
+      <c r="J72" s="8" t="s">
         <v>474</v>
       </c>
-      <c r="K72" s="10" t="s">
+      <c r="K72" s="8" t="s">
         <v>475</v>
       </c>
-      <c r="L72" s="10" t="s">
+      <c r="L72" s="8" t="s">
         <v>476</v>
       </c>
-      <c r="M72" s="10" t="s">
+      <c r="M72" s="8" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="73" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="9">
+    <row r="73" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="7">
         <v>21</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="B73" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="C73" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D73" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F73" s="9" t="s">
+      <c r="D73" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F73" s="7" t="s">
         <v>478</v>
       </c>
-      <c r="G73" s="9" t="s">
+      <c r="G73" s="7" t="s">
         <v>479</v>
       </c>
-      <c r="H73" s="9" t="s">
+      <c r="H73" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="I73" s="9" t="s">
+      <c r="I73" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="J73" s="9" t="s">
+      <c r="J73" s="7" t="s">
         <v>469</v>
       </c>
-      <c r="K73" s="9" t="s">
+      <c r="K73" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="L73" s="9" t="s">
+      <c r="L73" s="7" t="s">
         <v>482</v>
       </c>
-      <c r="M73" s="9" t="s">
+      <c r="M73" s="7" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="74" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="9">
+    <row r="74" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="7">
         <v>22</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="B74" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="C74" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D74" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F74" s="9" t="s">
+      <c r="D74" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F74" s="7" t="s">
         <v>484</v>
       </c>
-      <c r="G74" s="9" t="s">
+      <c r="G74" s="7" t="s">
         <v>485</v>
       </c>
-      <c r="H74" s="9" t="s">
+      <c r="H74" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="I74" s="9" t="s">
+      <c r="I74" s="7" t="s">
         <v>486</v>
       </c>
-      <c r="J74" s="9" t="s">
+      <c r="J74" s="7" t="s">
         <v>475</v>
       </c>
-      <c r="K74" s="9" t="s">
+      <c r="K74" s="7" t="s">
         <v>487</v>
       </c>
-      <c r="L74" s="9" t="s">
+      <c r="L74" s="7" t="s">
         <v>488</v>
       </c>
-      <c r="M74" s="9" t="s">
+      <c r="M74" s="7" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="75" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="9">
+    <row r="75" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="13">
         <v>23</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="B75" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C75" s="9" t="s">
+      <c r="C75" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="D75" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F75" s="9" t="s">
+      <c r="D75" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F75" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="G75" s="9" t="s">
+      <c r="G75" s="13" t="s">
         <v>490</v>
       </c>
-      <c r="H75" s="9" t="s">
+      <c r="H75" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="I75" s="9" t="s">
+      <c r="I75" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="J75" s="9" t="s">
+      <c r="J75" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="K75" s="9" t="s">
+      <c r="K75" s="13" t="s">
         <v>492</v>
       </c>
-      <c r="L75" s="9" t="s">
+      <c r="L75" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="M75" s="9" t="s">
+      <c r="M75" s="13" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="76" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="11">
+    <row r="76" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="9">
         <v>24</v>
       </c>
-      <c r="B76" s="11" t="s">
+      <c r="B76" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C76" s="11" t="s">
+      <c r="C76" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="D76" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F76" s="11" t="s">
+      <c r="D76" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E76" s="12"/>
+      <c r="F76" s="9" t="s">
         <v>494</v>
       </c>
-      <c r="G76" s="11" t="s">
+      <c r="G76" s="9" t="s">
         <v>453</v>
       </c>
-      <c r="H76" s="11" t="s">
+      <c r="H76" s="9" t="s">
         <v>495</v>
       </c>
-      <c r="I76" s="11" t="s">
+      <c r="I76" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="K76" s="11" t="s">
+      <c r="K76" s="9" t="s">
         <v>455</v>
       </c>
-      <c r="L76" s="11" t="s">
+      <c r="L76" s="9" t="s">
         <v>496</v>
       </c>
-      <c r="M76" s="11" t="s">
+      <c r="M76" s="9" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="77" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="5">
+    <row r="77" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="13">
         <v>25</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C77" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E77" s="5" t="s">
+      <c r="E77" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="F77" s="5" t="s">
+      <c r="F77" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="G77" s="5" t="s">
+      <c r="G77" s="13" t="s">
         <v>498</v>
       </c>
-      <c r="H77" s="5" t="s">
+      <c r="H77" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="I77" s="5" t="s">
+      <c r="I77" s="13" t="s">
         <v>499</v>
       </c>
-      <c r="J77" s="5" t="s">
+      <c r="J77" s="13" t="s">
         <v>446</v>
       </c>
-      <c r="K77" s="5" t="s">
+      <c r="K77" s="13" t="s">
         <v>500</v>
       </c>
-      <c r="L77" s="5" t="s">
+      <c r="L77" s="13" t="s">
         <v>501</v>
       </c>
-      <c r="M77" s="5" t="s">
+      <c r="M77" s="13" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="78" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="11">
+    <row r="78" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="9">
         <v>26</v>
       </c>
-      <c r="B78" s="11" t="s">
+      <c r="B78" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C78" s="11" t="s">
+      <c r="C78" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="D78" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F78" s="11" t="s">
+      <c r="D78" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F78" s="9" t="s">
         <v>503</v>
       </c>
-      <c r="G78" s="11" t="s">
+      <c r="G78" s="9" t="s">
         <v>460</v>
       </c>
-      <c r="H78" s="11" t="s">
+      <c r="H78" s="9" t="s">
         <v>504</v>
       </c>
-      <c r="I78" s="11" t="s">
+      <c r="I78" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="K78" s="11" t="s">
+      <c r="K78" s="9" t="s">
         <v>462</v>
       </c>
-      <c r="L78" s="11" t="s">
+      <c r="L78" s="9" t="s">
         <v>505</v>
       </c>
-      <c r="M78" s="11" t="s">
+      <c r="M78" s="9" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="79" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="9">
+    <row r="79" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="13">
         <v>27</v>
       </c>
-      <c r="B79" s="9" t="s">
+      <c r="B79" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="C79" s="9" t="s">
+      <c r="C79" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="D79" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F79" s="9" t="s">
+      <c r="D79" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F79" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="G79" s="9" t="s">
+      <c r="G79" s="13" t="s">
         <v>507</v>
       </c>
-      <c r="H79" s="9" t="s">
+      <c r="H79" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="I79" s="9" t="s">
+      <c r="I79" s="13" t="s">
         <v>508</v>
       </c>
-      <c r="J79" s="9" t="s">
+      <c r="J79" s="13" t="s">
         <v>488</v>
       </c>
-      <c r="K79" s="9" t="s">
+      <c r="K79" s="13" t="s">
         <v>509</v>
       </c>
-      <c r="L79" s="9" t="s">
+      <c r="L79" s="13" t="s">
         <v>510</v>
       </c>
-      <c r="M79" s="9" t="s">
+      <c r="M79" s="13" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="80" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="8">
+    <row r="80" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="6">
         <v>28</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="B80" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C80" s="8" t="s">
+      <c r="C80" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="D80" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F80" s="8" t="s">
+      <c r="D80" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F80" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="G80" s="8" t="s">
+      <c r="G80" s="6" t="s">
         <v>454</v>
       </c>
-      <c r="H80" s="8" t="s">
+      <c r="H80" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="I80" s="8" t="s">
+      <c r="I80" s="6" t="s">
         <v>474</v>
       </c>
-      <c r="J80" s="8" t="s">
+      <c r="J80" s="6" t="s">
         <v>512</v>
       </c>
-      <c r="K80" s="8" t="s">
+      <c r="K80" s="6" t="s">
         <v>513</v>
       </c>
-      <c r="L80" s="8" t="s">
+      <c r="L80" s="6" t="s">
         <v>514</v>
       </c>
-      <c r="M80" s="8" t="s">
+      <c r="M80" s="6" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="81" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="8">
+    <row r="81" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="6">
         <v>29</v>
       </c>
-      <c r="B81" s="8" t="s">
+      <c r="B81" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C81" s="8" t="s">
+      <c r="C81" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="D81" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F81" s="8" t="s">
+      <c r="D81" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F81" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="G81" s="8" t="s">
+      <c r="G81" s="6" t="s">
         <v>480</v>
       </c>
-      <c r="I81" s="8" t="s">
+      <c r="I81" s="6" t="s">
         <v>516</v>
       </c>
-      <c r="J81" s="8" t="s">
+      <c r="J81" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="K81" s="8" t="s">
+      <c r="K81" s="6" t="s">
         <v>517</v>
       </c>
-      <c r="L81" s="8" t="s">
+      <c r="L81" s="6" t="s">
         <v>518</v>
       </c>
-      <c r="M81" s="8" t="s">
+      <c r="M81" s="6" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="82" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="8">
+    <row r="82" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="6">
         <v>30</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="B82" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C82" s="8" t="s">
+      <c r="C82" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D82" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F82" s="8" t="s">
+      <c r="D82" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F82" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="G82" s="8" t="s">
+      <c r="G82" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="I82" s="8" t="s">
+      <c r="I82" s="6" t="s">
         <v>520</v>
       </c>
-      <c r="J82" s="8" t="s">
+      <c r="J82" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="K82" s="8" t="s">
+      <c r="K82" s="6" t="s">
         <v>521</v>
       </c>
-      <c r="L82" s="8" t="s">
+      <c r="L82" s="6" t="s">
         <v>522</v>
       </c>
-      <c r="M82" s="8" t="s">
+      <c r="M82" s="6" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="83" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="8">
+    <row r="83" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="6">
         <v>31</v>
       </c>
-      <c r="B83" s="8" t="s">
+      <c r="B83" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C83" s="8" t="s">
+      <c r="C83" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="D83" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F83" s="8" t="s">
+      <c r="D83" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F83" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="G83" s="8" t="s">
+      <c r="G83" s="6" t="s">
         <v>486</v>
       </c>
-      <c r="I83" s="8" t="s">
+      <c r="I83" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="J83" s="8" t="s">
+      <c r="J83" s="6" t="s">
         <v>525</v>
       </c>
-      <c r="K83" s="8" t="s">
+      <c r="K83" s="6" t="s">
         <v>526</v>
       </c>
-      <c r="L83" s="8" t="s">
+      <c r="L83" s="6" t="s">
         <v>527</v>
       </c>
-      <c r="M83" s="8" t="s">
+      <c r="M83" s="6" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A84" s="3">
+      <c r="A84" s="2">
         <v>32</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A85" s="3">
+    <row r="85" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="11">
         <v>33</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C85" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="D85" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F85" s="3" t="s">
+      <c r="D85" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F85" s="11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A86" s="3">
+    <row r="86" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="11">
         <v>34</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B86" s="11" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A87" s="3">
+    <row r="87" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="11">
         <v>35</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C87" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="D87" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F87" s="3" t="s">
+      <c r="D87" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F87" s="11" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A88" s="3">
+    <row r="88" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="11">
         <v>36</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C88" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="D88" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F88" s="3" t="s">
+      <c r="D88" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F88" s="11" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A89" s="3">
+    <row r="89" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="11">
         <v>37</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C89" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="D89" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F89" s="3" t="s">
+      <c r="D89" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F89" s="11" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A90" s="3">
+    <row r="90" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="11">
         <v>38</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="C90" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="D90" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F90" s="3" t="s">
+      <c r="D90" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F90" s="11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A91" s="3">
+    <row r="91" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="11">
         <v>39</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="C91" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="D91" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F91" s="3" t="s">
+      <c r="D91" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F91" s="11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A92" s="3">
+    <row r="92" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="11">
         <v>40</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B92" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="C92" s="3" t="s">
+      <c r="C92" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="D92" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F92" s="3" t="s">
+      <c r="D92" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F92" s="11" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A93" s="3">
+    <row r="93" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="13">
         <v>41</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B93" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C93" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="D93" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F93" s="3" t="s">
+      <c r="D93" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F93" s="13" t="s">
         <v>529</v>
       </c>
-      <c r="H93" s="3" t="s">
+      <c r="H93" s="13" t="s">
         <v>530</v>
       </c>
-      <c r="I93" s="3" t="s">
+      <c r="I93" s="13" t="s">
         <v>531</v>
       </c>
-      <c r="J93" s="3" t="s">
+      <c r="J93" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="K93" s="3" t="s">
+      <c r="K93" s="13" t="s">
         <v>496</v>
       </c>
-      <c r="L93" s="3" t="s">
+      <c r="L93" s="13" t="s">
         <v>482</v>
       </c>
-      <c r="M93" s="3" t="s">
+      <c r="M93" s="13" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C94" s="3" t="s">
+    <row r="94" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C94" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="F94" s="3" t="s">
+      <c r="F94" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="G94" s="3" t="s">
+      <c r="G94" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="I94" s="3" t="s">
+      <c r="I94" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="J94" s="3" t="s">
+      <c r="J94" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="K94" s="3" t="s">
+      <c r="K94" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="L94" s="3" t="s">
+      <c r="L94" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="M94" s="3" t="s">
+      <c r="M94" s="4" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A95" s="3">
+    <row r="95" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="13">
         <v>42</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C95" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="D95" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F95" s="3" t="s">
+      <c r="D95" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F95" s="13" t="s">
         <v>538</v>
       </c>
-      <c r="G95" s="3" t="s">
+      <c r="G95" s="13" t="s">
         <v>539</v>
       </c>
-      <c r="H95" s="3" t="s">
+      <c r="H95" s="13" t="s">
         <v>468</v>
       </c>
-      <c r="I95" s="3" t="s">
+      <c r="I95" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="J95" s="3" t="s">
+      <c r="J95" s="13" t="s">
         <v>524</v>
       </c>
-      <c r="K95" s="3" t="s">
+      <c r="K95" s="13" t="s">
         <v>540</v>
       </c>
-      <c r="L95" s="3" t="s">
+      <c r="L95" s="13" t="s">
         <v>541</v>
       </c>
-      <c r="M95" s="3" t="s">
+      <c r="M95" s="13" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A96" s="3">
+    <row r="96" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C96" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="H96" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="I96" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="J96" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="K96" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="L96" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="M96" s="4" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="2">
         <v>43</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B97" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C96" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="F96" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>543</v>
-      </c>
-      <c r="H96" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="I96" s="3" t="s">
-        <v>544</v>
-      </c>
-      <c r="J96" s="3" t="s">
-        <v>540</v>
-      </c>
-      <c r="K96" s="3" t="s">
-        <v>545</v>
-      </c>
-      <c r="L96" s="3" t="s">
-        <v>546</v>
-      </c>
-      <c r="M96" s="3" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="3">
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="2">
         <v>44</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B98" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" s="3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="2">
         <v>45</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B99" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="2">
         <v>46</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B100" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" s="11"/>
+      <c r="B102" s="2" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" s="3"/>
+      <c r="B103" s="2" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" s="12"/>
+      <c r="B104" s="2" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" s="8"/>
+      <c r="B105" s="2" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" s="6"/>
+      <c r="B106" s="2" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" s="7"/>
+      <c r="B107" s="2" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" s="5"/>
+      <c r="B108" s="2" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" s="13"/>
+      <c r="B109" s="2" t="s">
+        <v>554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>